<commit_message>
merged low (a,c) field with high tfp field
</commit_message>
<xml_diff>
--- a/paras_for_sensitivity.xlsx
+++ b/paras_for_sensitivity.xlsx
@@ -21,7 +21,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +155,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="33">
@@ -498,10 +503,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -823,19 +831,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1">
         <v>500000</v>
       </c>
@@ -869,21 +877,36 @@
         <f>EXP(J1-1)</f>
         <v>1</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <f>10^10</f>
         <v>10000000000</v>
       </c>
-      <c r="M1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1">
+        <v>2000</v>
+      </c>
+      <c r="P1" s="1">
+        <v>0.31994128399999999</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>51806.128900000003</v>
+      </c>
+      <c r="R1" s="1">
+        <v>13447412000</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2802.3725100000001</v>
+      </c>
+      <c r="T1">
+        <v>0.11014421377801099</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2">
         <f>0.5*A$1</f>
         <v>250000</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:G17" si="0">B$1</f>
+        <f t="shared" ref="B2:G15" si="0">B$1</f>
         <v>100000</v>
       </c>
       <c r="C2">
@@ -918,16 +941,31 @@
         <f>EXP(J2-1)</f>
         <v>0.53526142851899028</v>
       </c>
-      <c r="L2">
-        <f>L$1*$K2</f>
-        <v>5352614285.1899033</v>
-      </c>
       <c r="M2">
         <f>M$1*$K2</f>
+        <v>5352614285.1899033</v>
+      </c>
+      <c r="N2">
+        <f>N$1*$K2</f>
         <v>1070.5228570379807</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P2" s="1">
+        <v>0.32539639300000001</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>46243.251400000001</v>
+      </c>
+      <c r="R2" s="1">
+        <v>5239849240</v>
+      </c>
+      <c r="S2" s="1">
+        <v>923.43140500000004</v>
+      </c>
+      <c r="T2">
+        <v>0.115872493950051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3">
         <f>2*A$1</f>
         <v>1000000</v>
@@ -968,18 +1006,33 @@
         <f>EXP(J3-1)</f>
         <v>3.4903429574618414</v>
       </c>
-      <c r="L3">
-        <f>L$1*$K3</f>
-        <v>34903429574.618416</v>
-      </c>
       <c r="M3">
         <f>M$1*$K3</f>
+        <v>34903429574.618416</v>
+      </c>
+      <c r="N3">
+        <f>N$1*$K3</f>
         <v>6980.6859149236825</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P3" s="1">
+        <v>0.31170177199999999</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>64984.938099999999</v>
+      </c>
+      <c r="R3" s="1">
+        <v>28626857300</v>
+      </c>
+      <c r="S3" s="1">
+        <v>9431.5667099999991</v>
+      </c>
+      <c r="T3">
+        <v>8.9405409010305095E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4">
-        <f t="shared" ref="A4:G23" si="3">A$1</f>
+        <f t="shared" ref="A4:G21" si="3">A$1</f>
         <v>500000</v>
       </c>
       <c r="B4">
@@ -1006,8 +1059,43 @@
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I27" si="4">(A4-B4)*C4*B4</f>
+        <v>562500</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J27" si="5">I4/G4</f>
+        <v>0.5625</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K27" si="6">EXP(J4-1)</f>
+        <v>0.64564852642789206</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:N27" si="7">M$1*$K4</f>
+        <v>6456485264.2789202</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="7"/>
+        <v>1291.2970528557842</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.324619828</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>46276.619200000001</v>
+      </c>
+      <c r="R4" s="1">
+        <v>7800762130</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1433.2946300000001</v>
+      </c>
+      <c r="T4">
+        <v>0.11291934221189601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5">
         <f t="shared" si="3"/>
         <v>500000</v>
@@ -1036,8 +1124,43 @@
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <f t="shared" si="4"/>
+        <v>1500000</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>1.6487212707001282</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="7"/>
+        <v>16487212707.001282</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="7"/>
+        <v>3297.4425414002562</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.31892846400000002</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>51675.725899999998</v>
+      </c>
+      <c r="R5" s="1">
+        <v>20012207800</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4786.2320799999998</v>
+      </c>
+      <c r="T5">
+        <v>0.10070200547870201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6">
         <f>0.1*A$1</f>
         <v>50000</v>
@@ -1066,8 +1189,29 @@
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="5"/>
+        <v>0.01</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>0.37157669102204571</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="7"/>
+        <v>3715766910.2204571</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="7"/>
+        <v>743.15338204409147</v>
+      </c>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7">
         <f>0.01*A$1</f>
         <v>5000</v>
@@ -1076,676 +1220,1039 @@
         <f>0.01*B$1</f>
         <v>1000</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="C7" s="1">
         <f>100*C$1</f>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="D8">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E8">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F8">
+      <c r="F7">
         <f t="shared" si="0"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="5"/>
+        <v>0.01</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>0.37157669102204571</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="7"/>
+        <v>3715766910.2204571</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="7"/>
+        <v>743.15338204409147</v>
+      </c>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
         <f t="shared" si="3"/>
         <v>500000</v>
       </c>
-      <c r="B9">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C8" s="1">
         <f>10*C$1</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="D9">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E9">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F9">
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="4"/>
+        <v>10000000</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>8103.0839275753842</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="7"/>
+        <v>81030839275753.844</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="7"/>
+        <v>16206167.855150769</v>
+      </c>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
         <f t="shared" si="3"/>
         <v>500000</v>
       </c>
-      <c r="B10">
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C9" s="1">
         <f>0.1*C$1</f>
         <v>2.5000000000000002E-6</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="4"/>
+        <v>100000</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>0.40656965974059911</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="7"/>
+        <v>4065696597.4059911</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="7"/>
+        <v>813.13931948119819</v>
+      </c>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
       <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D11">
+        <v>0.6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D12">
+        <v>0.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D13">
+        <v>0.9</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C11" s="1">
-        <f>0.01*C$1</f>
-        <v>2.5000000000000004E-7</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D12">
-        <v>0.5</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D13">
-        <v>0.6</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D14">
-        <v>0.8</v>
-      </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D15">
-        <v>0.9</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>100000</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E16">
         <f>5*E$1</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F16">
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
         <f t="shared" si="3"/>
         <v>500000</v>
       </c>
-      <c r="B17">
+      <c r="B15">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="C17">
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D17">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E17">
+      <c r="E15">
         <f>2*E$1</f>
         <v>0.03</v>
       </c>
-      <c r="F17">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
         <f t="shared" si="3"/>
         <v>500000</v>
       </c>
-      <c r="B18">
+      <c r="B16">
         <f t="shared" si="3"/>
         <v>100000</v>
       </c>
-      <c r="C18">
+      <c r="C16">
         <f t="shared" si="3"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D18">
+      <c r="D16">
         <f t="shared" si="3"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E18">
+      <c r="E16">
         <f>0.5*E$1</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="F18">
+      <c r="F16">
         <f t="shared" si="3"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
         <f t="shared" si="3"/>
         <v>500000</v>
       </c>
-      <c r="B19">
+      <c r="B17">
         <f t="shared" si="3"/>
         <v>100000</v>
       </c>
-      <c r="C19">
+      <c r="C17">
         <f t="shared" si="3"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D19">
+      <c r="D17">
         <f t="shared" si="3"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E19">
+      <c r="E17">
         <f>0.2*E$1</f>
         <v>3.0000000000000001E-3</v>
       </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.3</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.5</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="3"/>
+        <v>100000</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.7</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>1000000</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <f t="shared" ref="A22:G27" si="8">A$1</f>
+        <v>500000</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="8"/>
+        <v>100000</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="8"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="8"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F22">
+        <v>0.8</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="8"/>
+        <v>1000000</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="7"/>
+        <v>10000000000</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="7"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <f t="shared" si="8"/>
+        <v>500000</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="8"/>
+        <v>100000</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="8"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="8"/>
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="8"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="8"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="3"/>
-        <v>100000</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="3"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="3"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F20">
-        <v>0.3</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="3"/>
-        <v>100000</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="3"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="3"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F21">
-        <v>0.4</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="3"/>
-        <v>100000</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F22">
-        <v>0.5</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="3"/>
-        <v>500000</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="3"/>
-        <v>100000</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="3"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="3"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F23">
-        <v>0.7</v>
-      </c>
       <c r="G23">
-        <f t="shared" si="3"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" ref="A24:G29" si="4">A$1</f>
-        <v>500000</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="4"/>
-        <v>100000</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="4"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="4"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="4"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F24">
-        <v>0.8</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="4"/>
-        <v>500000</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="4"/>
-        <v>100000</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="4"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="4"/>
-        <v>0.71199999999999997</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="4"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G25">
         <f>0.1*G$1</f>
         <v>100000</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="I23" s="2">
         <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>8103.0839275753842</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>81030839275753.844</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="7"/>
+        <v>16206167.855150769</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <f t="shared" si="8"/>
         <v>500000</v>
       </c>
-      <c r="B26">
-        <f t="shared" si="4"/>
+      <c r="B24">
+        <f t="shared" si="8"/>
         <v>100000</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="4"/>
+      <c r="C24">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="4"/>
+      <c r="D24">
+        <f t="shared" si="8"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="4"/>
+      <c r="E24">
+        <f t="shared" si="8"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="4"/>
+      <c r="F24">
+        <f t="shared" si="8"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G26">
+      <c r="G24">
         <f>0.5*G$1</f>
         <v>500000</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="I24" s="2">
         <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="7"/>
+        <v>27182818284.59045</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="7"/>
+        <v>5436.5636569180906</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <f t="shared" si="8"/>
         <v>500000</v>
       </c>
-      <c r="B27">
-        <f t="shared" si="4"/>
+      <c r="B25">
+        <f t="shared" si="8"/>
         <v>100000</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="4"/>
+      <c r="C25">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D27">
-        <f t="shared" si="4"/>
+      <c r="D25">
+        <f t="shared" si="8"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="4"/>
+      <c r="E25">
+        <f t="shared" si="8"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
+      <c r="F25">
+        <f t="shared" si="8"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G27">
+      <c r="G25">
         <f>2*G$1</f>
         <v>2000000</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="I25" s="2">
         <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>0.60653065971263342</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="7"/>
+        <v>6065306597.1263342</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="7"/>
+        <v>1213.0613194252669</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <f t="shared" si="8"/>
         <v>500000</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="4"/>
+      <c r="B26">
+        <f t="shared" si="8"/>
         <v>100000</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="4"/>
+      <c r="C26">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D28">
-        <f t="shared" si="4"/>
+      <c r="D26">
+        <f t="shared" si="8"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="4"/>
+      <c r="E26">
+        <f t="shared" si="8"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="4"/>
+      <c r="F26">
+        <f t="shared" si="8"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G28">
+      <c r="G26">
         <f>5*G$1</f>
         <v>5000000</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="I26" s="2">
         <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>0.44932896411722156</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>4493289641.1722155</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="7"/>
+        <v>898.65792823444315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27">
+        <f t="shared" si="8"/>
         <v>500000</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="4"/>
+      <c r="B27">
+        <f t="shared" si="8"/>
         <v>100000</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="4"/>
+      <c r="C27">
+        <f t="shared" si="8"/>
         <v>2.5000000000000001E-5</v>
       </c>
-      <c r="D29">
-        <f t="shared" si="4"/>
+      <c r="D27">
+        <f t="shared" si="8"/>
         <v>0.71199999999999997</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="4"/>
+      <c r="E27">
+        <f t="shared" si="8"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
+      <c r="F27">
+        <f t="shared" si="8"/>
         <v>0.56999999999999995</v>
       </c>
-      <c r="G29">
+      <c r="G27">
         <f>10*G$1</f>
         <v>10000000</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="4"/>
+        <v>1000000</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>0.40656965974059911</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="7"/>
+        <v>4065696597.4059911</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="7"/>
+        <v>813.13931948119819</v>
       </c>
     </row>
   </sheetData>
@@ -1762,12 +2269,12 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>0.5</v>
       </c>
@@ -1782,7 +2289,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <f>A$1</f>
         <v>0.5</v>
@@ -1800,7 +2307,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <f t="shared" ref="A3:D29" si="1">A$1</f>
         <v>0.5</v>
@@ -1818,7 +2325,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1836,7 +2343,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1854,7 +2361,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1872,7 +2379,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1890,7 +2397,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1908,7 +2415,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1926,7 +2433,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1944,7 +2451,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1962,7 +2469,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1980,7 +2487,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -1998,7 +2505,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2016,7 +2523,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2034,7 +2541,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2052,7 +2559,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2070,7 +2577,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2088,7 +2595,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2106,7 +2613,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2124,7 +2631,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2142,7 +2649,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2160,7 +2667,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2178,7 +2685,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2196,7 +2703,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2214,7 +2721,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2232,7 +2739,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2250,7 +2757,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>0.5</v>
@@ -2268,7 +2775,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>0.5</v>

</xml_diff>